<commit_message>
Fixed Excel sheet graph issue. Added and (hopefully) completed report.
</commit_message>
<xml_diff>
--- a/Mitchell_Lab8/TimingCSV.xlsx
+++ b/Mitchell_Lab8/TimingCSV.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EECS-560\Mitchell_Lab8\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="TimingCSV" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -301,7 +301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +432,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -734,7 +750,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -777,6 +793,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -785,7 +809,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -814,11 +838,19 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -896,26 +928,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -968,13 +980,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.37042E-2</c:v>
+                  <c:v>0.0137042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8713200000000001E-2</c:v>
+                  <c:v>0.0287132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2694600000000003E-2</c:v>
+                  <c:v>0.0626946</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.1299728</c:v>
@@ -984,21 +996,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$14:$D$21</c:f>
+              <c:f>TimingCSV!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>400000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1050,37 +1062,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.5100799999999998E-2</c:v>
+                  <c:v>0.0151008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3778200000000001E-2</c:v>
+                  <c:v>0.0337782</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7188199999999998E-2</c:v>
+                  <c:v>0.0771882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15836039999999998</c:v>
+                  <c:v>0.1583604</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$14:$D$21</c:f>
+              <c:f>TimingCSV!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>400000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1095,11 +1107,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-267650208"/>
-        <c:axId val="-267649120"/>
+        <c:axId val="2125872584"/>
+        <c:axId val="2125883016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-267650208"/>
+        <c:axId val="2125872584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,26 +1171,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1217,12 +1209,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-267649120"/>
+        <c:crossAx val="2125883016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-267649120"/>
+        <c:axId val="2125883016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,26 +1269,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1335,7 +1307,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-267650208"/>
+        <c:crossAx val="2125872584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,26 +1444,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1544,37 +1496,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.6500000000000001E-4</c:v>
+                  <c:v>0.000665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3348000000000001E-3</c:v>
+                  <c:v>0.0013348</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7138000000000002E-3</c:v>
+                  <c:v>0.0027138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0569999999999999E-3</c:v>
+                  <c:v>0.005057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$2:$D$9</c:f>
+              <c:f>TimingCSV!$D$14:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40000</c:v>
+                  <c:v>40000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,37 +1578,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.9020000000000003E-4</c:v>
+                  <c:v>0.0005902</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2075999999999999E-3</c:v>
+                  <c:v>0.0012076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5270000000000002E-3</c:v>
+                  <c:v>0.002527</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5927999999999993E-3</c:v>
+                  <c:v>0.0045928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$2:$D$9</c:f>
+              <c:f>TimingCSV!$D$14:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40000</c:v>
+                  <c:v>40000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1671,11 +1623,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-269032176"/>
-        <c:axId val="-269036528"/>
+        <c:axId val="2125922184"/>
+        <c:axId val="2125930856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-269032176"/>
+        <c:axId val="2125922184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,26 +1682,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1788,12 +1720,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269036528"/>
+        <c:crossAx val="2125930856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-269036528"/>
+        <c:axId val="2125930856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,26 +1785,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1911,7 +1823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269032176"/>
+        <c:crossAx val="2125922184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3109,15 +3021,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>952501</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>587376</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3138,16 +3050,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>881062</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>42861</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>474662</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3212,7 +3124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3247,7 +3159,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3424,7 +3336,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3434,22 +3346,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H5" sqref="D1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3475,7 +3387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3483,7 +3395,7 @@
         <v>6.8999999999999997E-4</v>
       </c>
       <c r="D2">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="E2">
         <f t="array" ref="E2">AVERAGE(IF(MOD(ROW(B1:B20),4)=1,B1:B20))</f>
@@ -3508,7 +3420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3517,7 +3429,7 @@
       </c>
       <c r="D3">
         <f>D2*2</f>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E3">
         <f t="array" ref="E3">AVERAGE(IF(MOD(ROW(B21:B40),4)=1,B21:B40))</f>
@@ -3539,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3548,7 +3460,7 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D5" si="0">D3*2</f>
-        <v>20000</v>
+        <v>200000</v>
       </c>
       <c r="E4">
         <f t="array" ref="E4">AVERAGE(IF(MOD(ROW(B41:B60),4)=1,B41:B60))</f>
@@ -3567,7 +3479,7 @@
         <v>2.5270000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3576,7 +3488,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>400000</v>
       </c>
       <c r="E5">
         <f t="array" ref="E5">AVERAGE(IF(MOD(ROW(B61:B80),4)=1,B61:B80))</f>
@@ -3595,7 +3507,7 @@
         <v>4.5927999999999993E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3603,7 +3515,7 @@
         <v>7.0100000000000002E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3611,7 +3523,7 @@
         <v>1.5294E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3619,7 +3531,7 @@
         <v>5.8799999999999998E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3627,7 +3539,7 @@
         <v>1.3466000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3635,7 +3547,7 @@
         <v>6.5099999999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3655,7 +3567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3663,7 +3575,7 @@
         <v>5.9599999999999996E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3671,7 +3583,7 @@
         <v>1.3505E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3679,11 +3591,11 @@
         <v>6.3299999999999999E-4</v>
       </c>
       <c r="D14">
-        <f>10*D2</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <f>0.1*D2</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3691,11 +3603,11 @@
         <v>1.5275E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D17" si="1">10*D3</f>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D15:D17" si="1">0.1*D3</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -3704,10 +3616,10 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3716,10 +3628,10 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3727,7 +3639,7 @@
         <v>6.4999999999999997E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -3735,7 +3647,7 @@
         <v>1.5592999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -3743,7 +3655,7 @@
         <v>5.7200000000000003E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -3751,7 +3663,7 @@
         <v>2.8930000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -3759,7 +3671,7 @@
         <v>1.431E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -3767,7 +3679,7 @@
         <v>3.3592999999999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3775,7 +3687,7 @@
         <v>1.219E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -3783,7 +3695,7 @@
         <v>2.8309000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3791,7 +3703,7 @@
         <v>1.238E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -3799,7 +3711,7 @@
         <v>3.3307000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -3807,7 +3719,7 @@
         <v>1.204E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -3815,7 +3727,7 @@
         <v>2.8781000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -3823,7 +3735,7 @@
         <v>1.3259999999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3831,7 +3743,7 @@
         <v>3.3326000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -3839,7 +3751,7 @@
         <v>1.168E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -3847,7 +3759,7 @@
         <v>2.8639999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -3855,7 +3767,7 @@
         <v>1.4040000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -3863,7 +3775,7 @@
         <v>3.4247E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -3871,7 +3783,7 @@
         <v>1.279E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -3879,7 +3791,7 @@
         <v>2.8906000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -3887,7 +3799,7 @@
         <v>1.2750000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -3895,7 +3807,7 @@
         <v>3.4417999999999997E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -3903,7 +3815,7 @@
         <v>1.168E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -3911,7 +3823,7 @@
         <v>6.0581999999999997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -3919,7 +3831,7 @@
         <v>2.6280000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -3927,7 +3839,7 @@
         <v>7.7868000000000007E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -3935,7 +3847,7 @@
         <v>2.5249999999999999E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -3943,7 +3855,7 @@
         <v>6.3340999999999995E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -3951,7 +3863,7 @@
         <v>2.7060000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -3959,7 +3871,7 @@
         <v>7.6258000000000006E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -3967,7 +3879,7 @@
         <v>2.4160000000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -3975,7 +3887,7 @@
         <v>6.3839999999999994E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -3983,7 +3895,7 @@
         <v>2.748E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -3991,7 +3903,7 @@
         <v>7.6461000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -3999,7 +3911,7 @@
         <v>2.617E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -4007,7 +3919,7 @@
         <v>6.3330999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -4015,7 +3927,7 @@
         <v>2.8270000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -4023,7 +3935,7 @@
         <v>7.7170000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -4031,7 +3943,7 @@
         <v>2.63E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -4039,7 +3951,7 @@
         <v>6.2378999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -4047,7 +3959,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -4055,7 +3967,7 @@
         <v>7.8184000000000003E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -4063,7 +3975,7 @@
         <v>2.447E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -4071,7 +3983,7 @@
         <v>0.12881999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -4079,7 +3991,7 @@
         <v>5.4209999999999996E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -4087,7 +3999,7 @@
         <v>0.174736</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -4095,7 +4007,7 @@
         <v>5.058E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -4103,7 +4015,7 @@
         <v>0.13808599999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -4111,7 +4023,7 @@
         <v>4.8809999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -4119,7 +4031,7 @@
         <v>0.15171999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -4127,7 +4039,7 @@
         <v>4.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -4135,7 +4047,7 @@
         <v>0.12273000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -4143,7 +4055,7 @@
         <v>4.9800000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -4151,7 +4063,7 @@
         <v>0.15446299999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -4159,7 +4071,7 @@
         <v>4.4929999999999996E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -4167,7 +4079,7 @@
         <v>0.120698</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -4175,7 +4087,7 @@
         <v>4.9249999999999997E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -4183,7 +4095,7 @@
         <v>0.15005199999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -4191,7 +4103,7 @@
         <v>4.4270000000000004E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -4199,7 +4111,7 @@
         <v>0.13952999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -4207,7 +4119,7 @@
         <v>5.078E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -4215,7 +4127,7 @@
         <v>0.160831</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -4223,18 +4135,23 @@
         <v>4.5059999999999996E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2">
       <c r="B100" s="1"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2">
       <c r="B132" s="1"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2">
       <c r="B136" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>